<commit_message>
Clean up gantt chart
</commit_message>
<xml_diff>
--- a/docs/gantt.xlsx
+++ b/docs/gantt.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27309"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\4. sem\PRGPRJ\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madsmarquart/Desktop/DTU/30010 Programming Project/PRGPRJ/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F71208EA-1D27-413A-880A-499656C3F8EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{990356F5-2B71-4E5E-8047-F1A48D2EE55F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,19 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>MVP</t>
   </si>
@@ -89,9 +82,6 @@
     <t>Design first two levels</t>
   </si>
   <si>
-    <t>!!report during development</t>
-  </si>
-  <si>
     <t>minigame</t>
   </si>
   <si>
@@ -122,20 +112,53 @@
     <t>Gustav</t>
   </si>
   <si>
-    <t>EXAM!</t>
-  </si>
-  <si>
-    <t>AT DTU??</t>
-  </si>
-  <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>At DTU?</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Labels:</t>
+  </si>
+  <si>
+    <t>Obligatory done</t>
+  </si>
+  <si>
+    <t>Feature freeze</t>
+  </si>
+  <si>
+    <t>Report deadline</t>
+  </si>
+  <si>
+    <t>Exam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +188,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +243,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -227,7 +274,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
@@ -235,8 +282,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -556,225 +606,229 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD238ED-F060-40FF-AF3C-EE45A4B271E6}">
-  <dimension ref="A1:R29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.59765625" customWidth="1"/>
-    <col min="3" max="4" width="3.73046875" style="8" customWidth="1"/>
-    <col min="5" max="8" width="20.59765625" customWidth="1"/>
-    <col min="9" max="9" width="4" style="7" customWidth="1"/>
-    <col min="10" max="10" width="20.59765625" customWidth="1"/>
-    <col min="11" max="11" width="4.1328125" style="8" customWidth="1"/>
-    <col min="12" max="12" width="4.06640625" style="8" customWidth="1"/>
-    <col min="13" max="13" width="20.59765625" customWidth="1"/>
-    <col min="14" max="14" width="4" style="7" customWidth="1"/>
-    <col min="15" max="17" width="20.59765625" customWidth="1"/>
-    <col min="18" max="18" width="3.6640625" style="7" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="5" width="3.6640625" style="7" customWidth="1"/>
+    <col min="6" max="10" width="20.6640625" customWidth="1"/>
+    <col min="11" max="11" width="4.1640625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="4" style="7" customWidth="1"/>
+    <col min="13" max="16" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>1</v>
+      <c r="C3" s="2"/>
+      <c r="F3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="J4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="J5" s="5" t="s">
-        <v>11</v>
-      </c>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="6"/>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E7" s="6" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="5" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="F8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="O8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="11"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="F9" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="G10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="G11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="G12" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="H13" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="H14" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="H15" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A19" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" t="s">
-        <v>31</v>
-      </c>
-      <c r="M29" t="s">
-        <v>31</v>
-      </c>
-      <c r="P29" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>31</v>
-      </c>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup paperSize="9" orientation="portrait" copies="3" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>